<commit_message>
Updated vets.gov xml spreadsheet
Former-commit-id: 8943175fb14a85067588d9d92f93a54be598ca3d
</commit_message>
<xml_diff>
--- a/design/content/VetsXMLSiteMap_2018-09-20.xlsx
+++ b/design/content/VetsXMLSiteMap_2018-09-20.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/vacolewana2/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/vacolewana2/Documents/GitHub/va.gov-team/design/content/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{7865A027-0A1A-D04B-BE8E-B39BABDB3E2D}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{2C6B470B-7101-E441-8C88-5909311E0AD5}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="27120" windowHeight="18260" xr2:uid="{77A04D6B-F00A-43EB-AEFA-05D3661E9022}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="559" uniqueCount="282">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="561" uniqueCount="283">
   <si>
     <t>https://www.vets.gov/playbook/human-centered-design/</t>
   </si>
@@ -872,6 +872,9 @@
   </si>
   <si>
     <t>Content Retire - Redirect</t>
+  </si>
+  <si>
+    <t>https://www.vets.gov/scorecard/</t>
   </si>
 </sst>
 </file>
@@ -1291,11 +1294,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F6862AED-6C5C-41DE-9996-7CB79D28C2B5}">
-  <dimension ref="A1:F271"/>
+  <dimension ref="A1:F272"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft"/>
+      <pane ySplit="1" topLeftCell="A258" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F272" sqref="F272"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0.2"/>
@@ -3526,6 +3529,14 @@
         <v>263</v>
       </c>
       <c r="B271" s="1" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="272" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A272" s="1" t="s">
+        <v>282</v>
+      </c>
+      <c r="D272" s="1" t="s">
         <v>264</v>
       </c>
     </row>

</xml_diff>